<commit_message>
commit the pipeline code mig
</commit_message>
<xml_diff>
--- a/src/pipeline/credentials.xlsx
+++ b/src/pipeline/credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hema\Documents\OnPrem_to_ADO_Pipeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hema\Documents\GitHub\DevOpsServer2020TOADO_Migration\src\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A50667-E644-4369-B015-450224896FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088A6BC3-34F9-4BBD-95CB-24B607571222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Base URL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>http://172.191.4.85/DefaultCollection</t>
   </si>
@@ -49,16 +46,52 @@
   </si>
   <si>
     <t>BqV9EbVuxxzXtmzEdtdTfevv1qZ3EQszfR410EtLL0TDvbwxMruhJQQJ99AKACAAAAAyb0Q7AAASAZDOBwc3</t>
+  </si>
+  <si>
+    <t>Source_URL</t>
+  </si>
+  <si>
+    <t>Target_URL</t>
+  </si>
+  <si>
+    <t>https://dev.azure.com/PLMigration</t>
+  </si>
+  <si>
+    <t>hemag</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>Target_Pat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -81,16 +114,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -285,54 +325,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" customWidth="1"/>
     <col min="3" max="3" width="61.36328125" customWidth="1"/>
     <col min="4" max="4" width="23.1796875" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="99.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://172.191.4.85/" xr:uid="{81C3B48E-B9AB-491A-870B-904A23A7832E}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C9E8C601-174D-45B8-9D84-22E858A4E55F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>